<commit_message>
added to piascy and history of dhopadhola
</commit_message>
<xml_diff>
--- a/History and customs of Jopadhola.xlsx
+++ b/History and customs of Jopadhola.xlsx
@@ -4,23 +4,31 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Acknowledgement and Dedication" sheetId="1" r:id="rId1"/>
     <sheet name="Chapter 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Chapter 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Chapter 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc71390804" localSheetId="0">'Acknowledgement and Dedication'!$A$2</definedName>
     <definedName name="_Toc71390808" localSheetId="1">'Chapter 1'!$A$2</definedName>
+    <definedName name="_Toc71392403" localSheetId="2">'Chapter 2'!$A$2</definedName>
+    <definedName name="_Toc71392404" localSheetId="3">'Chapter 3'!$A$2</definedName>
+    <definedName name="_Toc71397457" localSheetId="2">'Chapter 2'!$A$6</definedName>
+    <definedName name="_Toc71397458" localSheetId="2">'Chapter 2'!$A$14</definedName>
+    <definedName name="_Toc71397459" localSheetId="2">'Chapter 2'!$A$22</definedName>
+    <definedName name="_Toc71397460" localSheetId="2">'Chapter 2'!$A$28</definedName>
+    <definedName name="_Toc71397461" localSheetId="2">'Chapter 2'!$A$36</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="144">
   <si>
     <t xml:space="preserve">WACH MA CHAKO </t>
   </si>
@@ -203,6 +211,255 @@
   </si>
   <si>
     <t xml:space="preserve">Paka dhopadhola fuod ongoye kod ndiiko mere m’otire miluwo (Standard Orthography), amomiyo wach madit manitye i kitawo me i bino nwaŋo ni ndiiko mere okidho ka wire wire.  </t>
+  </si>
+  <si>
+    <t>Wok ndir ma jo Padhola jo konyo iye Wakoli, jo Ngaya jo mako rijo nge madwoŋ swa, to jo mito bino chulo kwor bothi jo, ni rupir ama jo miyo Wakoli oturo jo.</t>
+  </si>
+  <si>
+    <t>LWENY PA JO PADHOLA</t>
+  </si>
+  <si>
+    <t>Indir ma Adhola donjo i piny me onwaŋo ngoye ji man to rumachien ma oro chiegin mia aryo tundo mia adek, nono meg to chako bino gi kwinyo jo to gime kelo lweny.</t>
+  </si>
+  <si>
+    <t>Mono meg me paka jo Sewe ndirino jo wok yo thenge ma jwom Malawa yo Kenya, aka nono meg jo wok yo telin ma Misowa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bedo pa lweny me rumachien tek tek ama, bende nyutho ni chango onwaŋo piny me ongoye ji man. </t>
+  </si>
+  <si>
+    <t>Bedi ka ameno di Adhola gin jo konyalo bedo iiye majo kokutho jo lwenyo; kendo di Owiny gin di jo konyalo woth tundo yo Kenya korogye mako lweny gijo gineko jo iyo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lweny ma dongo chango obedo awichiel ama: </t>
+  </si>
+  <si>
+    <t>lweny kod jo Sewe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lweny kod jo Misowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lweny pa Wakoli yo Busoga </t>
+  </si>
+  <si>
+    <t>lweny kod jo Ngaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kod lweny pa Kakunguru ama gike, to lweny me abino tito kwome i Siro 5. </t>
+  </si>
+  <si>
+    <t>lweny go Omwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo Sewe me jo nyalo bedo jo Masai mandirino jo wotho wok yo Kenya ka jo kwayo dhok pajo odoko ka jo mito mayo ji gigipiny pa jo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I woth pajo me ama jo chombo iye i piny me. Obedo wor achiel to jo tundo yo Matindi to jo chako neko ji munwaŋo jo nitye kenyo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aka jino madit mere onwaŋo obedo nono jo Ramogi, amumiyo jo Ramogi jo wero kir pama ni “Sewe oneko yach ma Matindi kada g’operenje.”  </t>
+  </si>
+  <si>
+    <t>Sewe jowaŋo udi to jo neko ji madit kareno jo lwenyo g’asere kod tonge, to jo ay jo ringo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lweny me obwoka bwoka jo Padhola amumiyo jo konyalo yikirok gi lweny maber wori no.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To wok indirino to jo Padhola jo chako yikirok ri lweny, jo kunyo wugo kweth mabin jo kano iye mon kod nyithindho ka lweny otundo.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wugo me yado kis nono kunyo apa jo. </t>
+  </si>
+  <si>
+    <t>Kendo jo kunyo buche man thoko gine udi pajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To bin ka jo Sewe jo mwonjo jo i dye wor (jo Sewe yado jo kimit lweny odiochieŋ jo liwo jo wor ayino), to jo podho i buche me mu thoko udi, to jo Padhola jo bino nwoyo jo anwoya gi kenyo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To ndir man ka jo bino odiochieŋ ji gye jo donjo i wugo, to jo Sewe jo ngoye gi ji ma jo neki to jo waŋo udi to jo dok. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lweny pa jo Sewe ochando jo Padhola swa rupir ndirino nyaka jo chako lweny, aka fuod jo kotegino maber.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To kada ameno, ri rieko ma kunyo buche thoko udi jo nyalo neko jo Sewe Maditi mere, aka nyaka manok mudoŋ ti riemo riema jo kalo jwom Malawa, ti mayo jo kir dhok pajo. </t>
+  </si>
+  <si>
+    <t>Wok ndirino jo Sewe jo kodok jo dwoko lweny.</t>
+  </si>
+  <si>
+    <t>Jo Misowa me a Wagisu.</t>
+  </si>
+  <si>
+    <t>Lweny me obedo ni jo Misowa ama jo pen kwinyo jo Padhola to jo Padhola, rupir jo Sewe ndirino jo tieko fuonjo jo lweny to jo neko jo Misowa to jo riemo jo kir witelin ma yopiny pajo.</t>
+  </si>
+  <si>
+    <t>Rumachien jo Padhola bende jo mito ni jo kidhi kwinyo jo Misowa yo witelin pajo koro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To kada jo Misowa ndirino jo nyapi gi lweny, jo Padhola ri wach ma jo kuya gine idho got gi woth iye jo ko nyalo lweny maber gi limo gigipiny munwaŋo jo kidho rigo paka chiemo, dhoki kod nyir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jo temoye kadi kweth to jo dhiere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ri ameno to jo Padhola jo dhiro rijo Misowa wach ni jomak mere mungoye odoko lweny rupir jo dhiero jo turo jo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo Misowa bende jo yeyere gi wach me; to jo yiko romo ika bedo achiel giparo kwom gigipiny mu nwaŋo ramo jo thenge korin gi korin.  </t>
+  </si>
+  <si>
+    <t>I romo me jo Padhola kod jo Misowa gye jo tweyo kit chiemo gi riŋo to jo bino gine, to jo tedo to jo chiemo kanya achiel to jo mako mere kichutho.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wok ndirino to jo Padhola jo chwoko ka bedo ma piny pajo machango jo romo iye gi jo Misowa, ni Mere-kit makir pama i lwoŋo ameno. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kareno jo wacho ni kenyo amuwok iye mere ma chale kod kit chiemo mandirino jo tero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To rwooth achiel ma Busoga chiegin ikew kod jo Padhola, mi lwoŋo ni Wakoli to lwoŋo jo Padhola konyo go gi lweny gi Baganda (Jomagara) mu nwaŋo jo mwonjo go lweny gine i piny pere. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo Padhola bende jo kokwero rupir Wakoli owacho miyo jo nyir, chiemo kod ŋaŋo man mathindho thindho mandirino ongoye yo Padhola. </t>
+  </si>
+  <si>
+    <t>Kuma jo Padhola jo tundo, to jo lwenyo swa ri Wasoga to jo turo Jomagere ma ndirino jo Padhola jo chwoko jo ni jo Ngaya, to jo riemo jo wok i piny pa Wakoli.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To jo Padhola jo dwoko i piny pajo gi kemba ma Wakoli omiyo jo.</t>
+  </si>
+  <si>
+    <t>To hongo kadho moro to jo Ngaya jo bino mwonjo jo Padhola.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nen tipo (map) ma Padhola. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To munyo Padhola gye jowinjo ni jo Ngaya jo bino lweny to jo kidho rijo kuma onwaŋo jo yuomere iye, kajo wacho ni, “Wirooko!  Wirooko!  Widooma!  Widooma konon!” to jo chako neko jo Ngaya pa nyithindho winyini dho jwom ma pama i lwoŋo ni Wadama.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gi mumiyo jo Padhola turo jo Ngaya ma piyo piyo, rupir ndirino jo Ngaya jo lwenyo gi tonge madongo kod kwoot mathindho thindho, aka tonge no ripek mere dhano chore achora chiegin aka chwowo gimoro.  </t>
+  </si>
+  <si>
+    <t>To jo Padhola ndirino tonge pa jo mathindho aka jo bola bola gi bor to chwowo gimoro kada kochore ka bothe chiegin, aka kwoot pajo ndirino dongo ma geŋo jo maber.</t>
+  </si>
+  <si>
+    <t>Wok ndirino to jo Ngaya jokodok jo dwoko kwinyo jo Padhola.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To kende jo Ngaya majo ringo, ama jo kowo ri Kakunguru miseni pajo Padhola kod paka joturo jo; amumiyo Kakunguru bende obino rumachien chulo kwor mere (nen Siro 5).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kir jwom mu lweny iiye ti lwoŋo ni Wadama.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banyole ama chango jo Padhola jo chwoko ni Omwa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo me ajoger pa jo Padhola machon kendo lweny kod jo yado bedo chiegin kis dwe kareno jo gye jo mwonjere amwonja.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lweny me chango oasa lwenyirok yo kew yo thenge ma Buwesa, ma jo Padhola jo lwoŋo ni Wesa, yo Senda kod yo Paya. </t>
+  </si>
+  <si>
+    <t>Yado ka jo Padhola jo neno ni dwe opor aka chingi dwe marachuch amuŋiyo malo to jo kidho mwonjo Omwa ni rupir ndirino silwany apa jo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lweny ma kite me otero hongo ma lach swa to kelo kwoor ma dwoŋ tek tek bothi jo Padhola kod Banyole. </t>
+  </si>
+  <si>
+    <t>Tundo pama, mere odoko dwoko bothi jo munyo jo nywomere kir gi nywomirok mungoye dhaw moro gye.</t>
+  </si>
+  <si>
+    <t>To ka dwe opor ma chinge maracham amutiŋere malo meno iwacho ni otiŋo chingi Omwa malo ko mwonji jo kosa kajo amajo mwonjo jo Padhola, jo amajo turo lweny no.</t>
+  </si>
+  <si>
+    <t>Kareno gima dwoŋ chango jo Padhola jo mito mayo jo chiemo pajo, rupir jo Padhola i hongo ma yochien munyo jo ŋiyo gi lweny tek tek jo kodok jo bedo jo fur madongo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To wok ibino pa Kakunguru chiegin yo oro 1890, lweny me kodok obedo kada dichiel.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To jo chwoko jo Padhola ni Badama, ka jo kwanyo kwom wach machango jo Padhola jo wacho rijo ni “Widoma”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kutho jo Ngaya jo neko jo Padhola madit kod waŋo udi rupir jo liwo aliwa jo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indir ma jo Padhola jo tieko lwenyo lweny aryo madongo apa jo Sewe kod apa jo Misowa, to nyingi jo chako winjirok kir wiloka man. </t>
+  </si>
+  <si>
+    <t>OGUTI LOKERE JA PADHOLA</t>
+  </si>
+  <si>
+    <t>To tho i oro 1912.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ri kayo chinge machango wode okayo. </t>
+  </si>
+  <si>
+    <t>Ndir munyo Oguti oneno ni lim pere dit, aka iyadech ma Pokoŋo onyo diny rigo to kwayo jo dongo pere ti yeyogo chorirok yo Tororo kuma chango nitye jonono Bendo pere man madit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oguti chango obedo dhano munywol go yo thenge ma Kachumbala i Teso District; aka yo koro bende ama go owok iye aka owotho to donjo i Padhola. </t>
+  </si>
+  <si>
+    <t>Gimo oriemo Oguti yo thugin won kiŋeyere, to ginago ripo bedo gimadwoŋ swa mumiyo go okun kichutho wok bothi wade pere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ndirino Oguti onwaŋo fuod nyiyach muripo ripo.  Gime otimere yo Nagongera iyadech ma Pokoŋo.</t>
+  </si>
+  <si>
+    <t>Munyo onen ni Oguti nyath maber, ryeki aka odoko nitye kod men, to jo dongo jo chokere to jo penjo go kole ka mito lokirok ja Padhola kosa onyo mito dok yo thugin.</t>
+  </si>
+  <si>
+    <t>To go kwero ni kinyal odoko dok wok paka chango jo thugin jotieko riemo go.  Ri ameno titero Oguti i migam to kwoŋere iye ka wacho ni otieko lokirok ja Padhola kichutho, ti lamo go imigam no, ti gwero go kod yen malweny.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milweni to nywomo ri Oguti mon adek: Abotha meno obedo nyaja Ramogi, kod Nyagoli gi Nyakuya nyir Morwa Sule. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jo Padhola to jo mito Oguti swa riwach ma men pere yo lweny, mayado go asa lwenyo gi men pere gye</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kendo ri kiyaka mayado iyaka gigipiny yo lweny, Oguti bende chango oyaka dhok madit yo lweny to kelo rigo ŋaŋo gi medo nywomo mon madit swa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wok ndirino to lokere nyath ma pecho kendo ma ja Padhola, to chako lwoŋo Owaro ni Omini aka Milweni kod mini Owaro to jo bedo baa mere kod mini.  </t>
+  </si>
+  <si>
+    <t>Rumachien munyo Oguti oŋaŋ to kwayo jo nono pere ni oyey go lwoŋo ye jo thugin man bende jo obin jo bed gine i Padhola.</t>
+  </si>
+  <si>
+    <t>Me achako bino pa ji mawok yo District ma Teso donjo i Padhola</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ka, amunyo ji man majo wok thenge ma Kenya aka jo winjereye dhodhok kod ji ma chango Oguti oomo jo yo Teso, bende to jo chako bino pere pa jagin pere.</t>
+  </si>
+  <si>
+    <t>Ti yeyere gine to kelo jo thugin man to jono bende jo lokere jo Padhola ma nono jo pa Bendo. .</t>
+  </si>
+  <si>
+    <t>Ji me bende to jo Padhola yeyere gijo bedo, ti chwoko nyingi jo ni Omia rupir chango jo wok yo thenge ma Kenya milwoŋo ni Mumias.</t>
+  </si>
+  <si>
+    <t>To Oguti iloko go bedo ja dwoŋ pajo, kareno imito ni go amunyuth ji me kula kod tim ma Padhola.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ji me bende to jo lokere jo Padhola kichutho, to jo chako nywomo nyir jo Padhola gi donjo i nonin ma Padhola mu pokere opokere.</t>
+  </si>
+  <si>
+    <t>nen Siro 5</t>
+  </si>
+  <si>
+    <t>Ri ŋeyirok machango Oguti oŋeyere iye yo lweny, munyo Kakunguru otieko turo piny me aka onyo iketho rwodhe Oguti bende timiyo bedo rwoth .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ja Bendo milwoŋo ni Milwen omunwaŋo Ogut i ger dhoki wor wor to dimo go to tero go pecho pere, to ketho go i oti padhako pere milwoŋo ni min Owaro. </t>
   </si>
 </sst>
 </file>
@@ -251,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -268,6 +525,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -913,12 +1189,470 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="69.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45">
+      <c r="A3" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30">
+      <c r="A4" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30">
+      <c r="A5" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45">
+      <c r="A6" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30">
+      <c r="A14" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30">
+      <c r="A16" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="30">
+      <c r="A17" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30">
+      <c r="A18" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="30">
+      <c r="A19" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="45">
+      <c r="A21" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="30">
+      <c r="A23" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="30">
+      <c r="A24" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="45">
+      <c r="A25" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="45">
+      <c r="A28" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="30">
+      <c r="A29" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="45">
+      <c r="A30" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="30">
+      <c r="A31" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="30">
+      <c r="A33" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="30">
+      <c r="A34" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="30">
+      <c r="A35" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="30">
+      <c r="A36" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="30">
+      <c r="A37" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="45">
+      <c r="A38" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="30">
+      <c r="A39" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="45">
+      <c r="A41" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="45">
+      <c r="A42" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="30">
+      <c r="A46" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="45">
+      <c r="A48" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="60">
+      <c r="A49" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="45">
+      <c r="A51" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="45">
+      <c r="A52" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="30">
+      <c r="A54" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="30">
+      <c r="A55" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="45">
+      <c r="A56" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="30">
+      <c r="A57" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="45">
+      <c r="A58" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="30">
+      <c r="A59" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="30">
+      <c r="A60" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="30">
+      <c r="A61" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="68.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45">
+      <c r="A3" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45">
+      <c r="A4" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45">
+      <c r="A5" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45">
+      <c r="A7" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30">
+      <c r="A8" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45">
+      <c r="A9" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="60">
+      <c r="A10" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30">
+      <c r="A11" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30">
+      <c r="A12" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="45">
+      <c r="A13" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30">
+      <c r="A14" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30">
+      <c r="A16" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="30">
+      <c r="A17" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30">
+      <c r="A18" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="45">
+      <c r="A20" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="45">
+      <c r="A22" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the rest of History of Jopadhola. Not clean
</commit_message>
<xml_diff>
--- a/History and customs of Jopadhola.xlsx
+++ b/History and customs of Jopadhola.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Acknowledgement and Dedication" sheetId="1" r:id="rId1"/>
     <sheet name="Chapter 1" sheetId="2" r:id="rId2"/>
     <sheet name="Chapter 2" sheetId="3" r:id="rId3"/>
     <sheet name="Chapter 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Chapter 4" sheetId="5" r:id="rId5"/>
+    <sheet name="The rest" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc71390804" localSheetId="0">'Acknowledgement and Dedication'!$A$2</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="166">
   <si>
     <t xml:space="preserve">WACH MA CHAKO </t>
   </si>
@@ -460,6 +462,72 @@
   </si>
   <si>
     <t xml:space="preserve"> Ja Bendo milwoŋo ni Milwen omunwaŋo Ogut i ger dhoki wor wor to dimo go to tero go pecho pere, to ketho go i oti padhako pere milwoŋo ni min Owaro. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paka ichowo Bura nen Adech III, Siro 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To chowo Bura gikenyo; to wok ndirino to Majanga bedo ja tel ma chowo Bura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bura bedo i tele man yo Nyawiyoga</t>
+  </si>
+  <si>
+    <t>Yado chon onwaŋo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kumo okel gigipiny me totero jo yo lul Tewo (Nyakiriga) towacho rijo ni me atele ma kabedo manyien pa Bura </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To munyo onwaŋ, ti penjo kumago owok iye, to kwero wacho rijo kwanyo woko ni kajo kelo rigo koŋo kod wot gwendi</t>
+  </si>
+  <si>
+    <t>I wacho ni nitye ndir ma Majanga orwenyo makinen tieko ndelo maromo abiriyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ri ameno to ji gye chako lworo Majanga gi miyogo dwoŋ gi winjo wach pere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  I lweny bende yado kowacho ni kidh win kumanyo, ko kidh thenge no tituro lweny, to kowacho ni kononi kada wikidho i bino turo win, apaka bende bedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Odoko ruman owacho ri ji ni nitye ogwaŋ Kwach neko nyako moro ka moro, ka ni kidho kenyo onwaŋ nyako no otieko kir tho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wadi jo ko yeyo; to rigiraura madwoŋ ka ni kidho poyo, Nyielo to neko ŋato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Obedo ndir moro kuma jo kidho dwar, Majanga owacho ni nyawoti gin achiel Nyielo ya neko</t>
+  </si>
+  <si>
+    <t>To wok chon chango Majanga oneno paka nitye kod gi moro iwiye pa jwok, ma kowacho ni gi moro ya timere to gino timere atima ameno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To rupir chango baa mere otii aka ja chandi, omin baa mere mi lwoŋo ni Akure amunywomo rigo; kareno kutho Majanga odongo pere kakwayo rigo dhoki aka omito go swa pa nyath pere won</t>
+  </si>
+  <si>
+    <t>Majanga chango baa mere i lwoŋo ni Kinara ja Nyapolo Ogule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kendo chango obedo ja lweny mamisen swa, ama bin telo kir ji yo lweny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kir Akisili gye (nen Adech III, Siro 8), to bedo jatel mere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To kada ameno otemo wacho ri jii ni joyikere ri lweny no; to rupir jo nicha chango jo lwenyo gi mundu amumiyo otur jo ma piyo piyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rumachien pa bino pa Kakunguru, Majanga obedo hongo manok to tho i oro chiegin 1905</t>
+  </si>
+  <si>
+    <t>SIRO 5</t>
+  </si>
+  <si>
+    <t>Majanga to limo dwoŋ madit ri kwom gigipiny me gye</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ndiri ma Kakunguru donjo i piny me gi turo, onwa?o Majanga onyo obedo jadwoŋ m'oti</t>
   </si>
 </sst>
 </file>
@@ -841,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -1039,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1191,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1520,7 +1588,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1655,4 +1723,146 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:A23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="63.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
100 more sentences to History
</commit_message>
<xml_diff>
--- a/History and customs of Jopadhola.xlsx
+++ b/History and customs of Jopadhola.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="300">
   <si>
     <t xml:space="preserve">WACH MA CHAKO </t>
   </si>
@@ -528,6 +528,408 @@
   </si>
   <si>
     <t xml:space="preserve"> Ndiri ma Kakunguru donjo i piny me gi turo, onwa?o Majanga onyo obedo jadwoŋ m'oti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To gavumenti paka tero gimoro moth, jo liŋa aliŋa gi ywak me tundo 14 September, 1936, ma Bwana District Commissioner, Budama, mandirino bedo Tororo ochoko jo Padhola to wacho rijo ni onyo pama joyeyere dimo dhano pajo won obedi ja Saza kandelo 23 September 1936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To jo chako kwayo gavumenti ni omiy jo ja Saza ma ja Padhola won</t>
+  </si>
+  <si>
+    <t>Wok i oro chiegin 1925 jo Padhola joneno ni jo oli dhumirok gi jowiloka paka Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To Kiwanuka bedo ja dwoŋ adhum marapena bedo i tindi mar'adhum ma Kisoko</t>
+  </si>
+  <si>
+    <t>Wok i oro 1929-1930, jo dongo Adhum jo paro wiro tindi mar'adhum kwanyo Nagongera tero Robongi mu par ni adier piny, to rumachien ti dok i geto Kisoko ayino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To munyo okowi Kiwanuka yo Padhola to Ali Afende Awor to lunjo kabedo pere paka Agent ma Samia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ndiri munyo oketh Eria Nsubuga bedo Agent ma Padhola Rasito Mayanja bende oketh bedo Agent ma Bunyole, aka Mikairi Kiwanuka Agent ma Samia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo Eriya oweyo tich to ja Magara man mi lwoŋo ni Mikairi Kiwanuka to bino lunjo ka bedo pere yo Nagongera paka Agent ma Padhola ioro 1928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To tho i oro 25 May 1956; kareno go ja oro 99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kenyo amu wok iye to dok yo piny pajo yo Pamagara i oro February 1952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To kidho i oti pere machango ogeto Bira, rumachien to tuki i oti pere man yo Mulanda</t>
+  </si>
+  <si>
+    <t>I oro 1927, Eria okwayo ywomirok wok i tich maradhum; ndirino Wasungu weg jo tieko nia? ipiny me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka bin rwodhe jo Gombila i dimo jo tich paka ja Saza mathumo banjin dwe achiele chiele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To wok ndirino kodok oketh ja Saza, to bin Eria won bedo paka Agent ma Padhola aka odoko bedo paka ja Saza mere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jo Nyapolo to jo osa go both Eria, titweyo go yo lweny, to tho gi yo Kisumu i oro 1917</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mission pama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To gimo mieno go, to ere mito nyako ma nyamin Oloo Majanga milwoo ni Nyaruwa, munwaŋo fuonjere pa Perikeki ndir munyo nyaka jo tundo Nagongera kumanitye </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To odoko Eria onwaŋo paro ketho ja pa Bendo mandirino ja Gombila ma Nagongera ma magere ndirino jo chwoko nyinge ni Sabakaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To jo Nyapolo jo ko yeyo, kajo wacho ni dwoŋ no apa jo kiripi nono man odoko obed iiye</t>
+  </si>
+  <si>
+    <t>Ndiri munyo oriem Oloo Majanga, onwaŋo Eria paro ketho Okech Okeya lunjo ka bedo no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Koro amudwoko iye to bedo nyaka math to tho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To munyo oriem Oloo, to piny gye jo kwero winjo adhum, ri ameno ti mako go tikidho i tweyo go Jinja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ri ameno to magere jo riemo go iyadhum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Omito ni ji pere jo obedi i siem manya chon, ma medho amedha kod kisangala</t>
+  </si>
+  <si>
+    <t>Oloo chango ger, aka komito kite adhum manyien me ma magere jo kelo</t>
+  </si>
+  <si>
+    <t>To, Oloo Majanga konyalo tiyirok kod Eria, ka wacho ni, "Wendo awenda kinyal dhuman, kosa oran ni maki ŋatin mungoye wach ma ŋato otimo; ni kole ka ja Magara no mito chiemo owach adhir rigo chiemo to ma kiwene dhuman pa jago pere!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Eria Nsubuga won kod Oloo Majanga ndiri no jo bedo Nagongera, amubedo, tindi maradhum madwoŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kendo kis rwoth me yado tiyo kod jo magere ma jo konyo go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jome ama jo bedo rwodhe marapena, to rumachien odoko okidhi ki baro dier Gombilin 1oko mathindo thindho ti medo ketho rwodhe man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To Gombolin mere ti ketho ji me: Okech Okeya, Mulanda; Oloo Otaba, Nyawiyoga; Oguti, Tororo aka munyo otho to Samwiri Dinga lunjo, rwoth pere; Palinyaŋ Merikiti kod Molo, aka munyo onek go to Makode lunjo ka pere; Oluli; omin Palinyaŋ Kidoko, aka munyo otho tiketho ja Mugwere mi lwoŋo ni Mulyambuzi; Kayinja Majanga, Nagongera, kodi Kirewa; kod Owondo, Kwapa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Oloo Majanga mu bedo wod pa ŋata chango oŋeyere tek tek i gigipiny me gye, ti miyo go bedo paka ja Saza, matero rwodhe wad gye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Eria open tiyirok kod jo dongo Bura, jodongo Akisili kod jo dongo machango jo telo lweny, ama go okutho omiyo jo bedo jo radhum pere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To ketho jali milwoŋo ni Eria Nsubuga telo adhum maPadhola; ndirino i lwoŋo go ni Agent ma Padhola, to Kakunguru won dok yo Mbale</t>
+  </si>
+  <si>
+    <t>Munyo Kakunguru otieko turo Padhola to chako ketho adhum makite ma yo pajo yo Buganda, kareno yiko yo ri adhum pa Bungereza (British)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To jo chako kwoŋirok kod lweny gi Magere majo lwenyo kod mach!  Ndirino ja lweny machon madwoŋ, Majanga, onwaŋo fuod nitye to kareno go otii tek tek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jo Padhola ma chuka chiene onwaŋo fuod ko tur jo i lweny moro gye, rume ama otur atura jo kichutho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jo donjo i piny me chiegin i oro 1890, to jo Padhola jo Chwoko jo ni Magere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Go aja Waganda machango owotho gi wadi aka jo turo piny ma Eastern Province ri adhum pa jo makwar; ndirino jo lwenyo kod mundu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Me abino pa Semei Kakunguru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To rumachien ma oro kweth to wach winjere ni nitye kweth mudoko bino, aka jonago jo lwenyo gi gimaneko aneka dhano gi bor aka Odoko mor swa, ni jonago jowok yothenge ma Misowa kod Bugwere</t>
+  </si>
+  <si>
+    <t>Wok chuka tur lweny pa jo Ngaya jo Magere jo dok jo ko bino lweny kod jo Padhola</t>
+  </si>
+  <si>
+    <t>PADHOLA KOD ADHUM 1890-1958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Yo Samia tiketho ja Saza pajo marapena Samisoni Were mariwo Samia kod Bugwe, mu chwoki nyinge ni Samia-Bugwe</t>
+  </si>
+  <si>
+    <t>To i oro 1947, wach ma Sazin to odoko dwako</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  I oro no won 1944, Ezekeri Kageni ma Bugwere Division to tich pere chungo; tiketho Danieri Mutaki i kabedo pere aka Paulo Sisye bedo Deputy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  I oro 1944, Andereya Obeli ma Tororo Division to tich pere chungo; tiketho Eria Ochieno ikabedo pere aka Semei Obonyo bedo Deputy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To wok iiye chani man manyien</t>
+  </si>
+  <si>
+    <t>Pok adhum me okidho maber tundo i oro 1944, ama nywowirok madit dit odonjo iiye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ti turo jo Sazin gye munwaŋo jo nitye i Tororo Division kod Bugwere Division, tiweyo jo Gombilin kod jo dongo me kende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka Danieri Mutaki ama luwo Ezekeri Kageni paka Deputy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bugwere kod Bunyole ti lwoŋoni Bugwere Division; aka rwoth matero jo gye tiketho Ezekeri Kageni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Eria Ochieno to bedo ŋata luwo Andereya Obeli paka Deputy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ti lwo?o Tororo ni Tororo Division; amanyo tero Budama kod Samia, aka rwoth matero jo gye tiketho Andereya Obeli</t>
+  </si>
+  <si>
+    <t>Ndir ma lweny ma 1939-1945, otundo gavumenti owiro adhumbe manitye iyadech mathurin: 1941 onwaŋ District machango i lwo?o ni Budama District, kareno tindi mere bedo Tororo, tiriwo kod Central District machango wok i oro 1937 oriwo Bugwere District kod Bugisu District; ti lwo?o jo ni Mbale District aka tindi mere to bedo Mbale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ri ameno ka 17 December 1938, to jo oro jomikwenda pajo kidho nenirok kod Chief Secretary, yo Entebbe, ka jo piemo ri wach me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To jo Padhola jo guti swa riwach ma baro adhumi pajo, gi thenge man miyo wendo pajo tero Saza mere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gigipiny me otimere ka 23 November 1938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka thenge man, ti lwoŋo ni East Budama tiketho Daudi Kakunguru bedo ja Saza mere</t>
+  </si>
+  <si>
+    <t>Ri ameno to gavumenti, baro adhum ma Padhola diryo, thenge man ti lwoŋo ni West Budama tiketho Andereya Obeli wod pa Majanga bedo ja Saza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wok i hongo no to wach me chungo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To jo Padhola jo koyeyere gine, kiri ndir munyo Provincial Commissioner ma Eastern Province obino Kisoko bino ketho Dinga i kom jo goyo motoka pano pajo kedho woko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To onwaŋo i ketho go bedo ja Saza ma Padhola i oro 1938</t>
+  </si>
+  <si>
+    <t>To gavumenti paro tek tek i kite ma turo teko me gye; ri ameno to idimo dhano ma kanywola ma Padhola to kareno otieko bedo i Padhola hongo malach wok thino pere gye aa, Samwiri Dinga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka teko ma pokirok dini, to bende donjo iiye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ji machango jo Padhola oyeyo jo bedo i Padhola paka wendo pajo, majo chwoko jo ni Omia (nen Siro 3), to jo bende jo chako piem ni dhano pajo amaripo tero Saza ma Padhola</t>
+  </si>
+  <si>
+    <t>Wooro pa rwodhe makis ja Gombila mito ni go ama wodim bedo ja Saza, to jo kelo nyuowo wiy ji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To teko mudoko bino ame, riwach ma pa ŋata odim tero Saza:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To indir ma Magere jo donjo to jo chako dhumo Padhola (nen Adech I, Siro 5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jodongo ma kite me amayido jo choko ji pajo kosa jotito riji pajo ka lweny kosa dwar obino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To kareno jadwoŋ ma oti man kidhum jadwoŋ ma oti man; kosa dhumo nono no gipi</t>
+  </si>
+  <si>
+    <t>Chango chon kis oti manono bedo kod jadwoŋ mere maneno gigi piny matimere i oti no</t>
+  </si>
+  <si>
+    <t>Me agigipiny madongo aryo machango asa poko nono ma kada onwaŋo obedo achiel to poko jange mumore to jo chako kir nywomirok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ra'meno konyo oti makoneko dhano no, kajo winjo ni joweg dhano jo liwo jo machulo kwor, to jo chako kwedirok kajo wacho ni, "Athu denge wikiri wichul kwor bothi wan ayino, kidha kidha win yo paŋadin won majo neko dhano mewin, ŋey win ni wakinono gi jono de be, wajo paŋadin riwan!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rupir chango manyachon ka nono man oneko dhano ma nono man, jowegi dhano monekino bende jobino to jo liwo dhano manono no kada ka moro to jo neko; meno achulo kwor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Mararyo, kwor, me chango wok ka oti man jo kwinyo aka joneko ji manono man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wangi bende kawaneko mawan wakiyaŋere gi jo de be!"</t>
+  </si>
+  <si>
+    <t>Ri ameno jomo thwonijo to jo mako nge to jo dhaw kajo wacho ni, "Aneni win jopaŋadin paka jodak wan aka onyo jo kwedo wan riwach riŋo ariŋa, onyo wok pama apee!  Wapokere apoka swa, wakinono gi jo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Amawok iye oti man jochako thwono jowotigin riŋo kajowacho ni "Wajo pa ŋadin riwan lokere wanono giwin mawayaŋere riŋo?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Marapena, dhaw kod akwedi, me chango wok kwom poriŋiŋo kosa lee munyo ko nek, kipoko to kirom ka pecho kosa nono lach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gima chango kelo pokirok me obedo ama:</t>
+  </si>
+  <si>
+    <t>To kareno inonini madongo no nitye paka nono Amor kod wad man odoko jopokere kinde mumore to doko jo chako nywomirok kada chango onwaŋo jo nono achiel kende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Giranena, paka nonini me: Lemera, Nyangwe, Wi-kenge kod Wi-lego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Manyutho ni jobedo jangi nonini man madongo aka jopokere kwomijo ihongo mafuod kokadho malach</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nitye nonini meg mathindho thindho mafuod kiŋeyere maber</t>
+  </si>
+  <si>
+    <t>I Padhola pama nitye nonini pyero aryo kod aryo madongo</t>
+  </si>
+  <si>
+    <t>To kiyot ŋeyo ni ji ma mon me jonywolo won ajomene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kiri pama nono meg paka Amor p'Olam, Amor Patikidiegi kod Amor Mugulu-Kasede, jopako nyingi mon me kajowacho ni, "Won piny Nyajurya kod Oryaŋ"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mon me jo nyalo bedo ni chango jo bedo mon pa Adhola won, amumiyo nyingi jo oasa wok malo bende loyo mon wadi jo machango jonitye ikitipa no</t>
+  </si>
+  <si>
+    <t>Parere ni ikitipa pa Adhola chango nitye mon aryo madongo, Nyajura kod Oryaŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Amumiyo kisi nono no bende lwoŋo Adhola ni baa jo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  I ji me amowok iye nonini gye manitye Padhola pama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rupir go amubedo jadwoŋ pajo kendo ja tel pajo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ji me meg chango nyithindho pere won monywolo, meg wutiminigo meg wade pere; to kareno jogye jo lwoŋo Adhola ni baa jo</t>
+  </si>
+  <si>
+    <t>Adhola paka atito iy'adech marapena, chango owotho kod ji pere</t>
+  </si>
+  <si>
+    <t>WACH MATITO ADECH MARARYO</t>
+  </si>
+  <si>
+    <t>ADECH II</t>
+  </si>
+  <si>
+    <t>MAPO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ri ameno to gavumenti thwono jo gye to loko tindi Mbale bedo District machowere ka kende</t>
+  </si>
+  <si>
+    <t>Gimokelo poko tindi ma Mbale bedo paka District mu pokere ka kende aa rupir obedo piem i dier Bukedi kod Bugisu, kareno kis ŋata achiel kwom jo mitoni tindi ma Mbale odoki yo District pajo ayino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka adech matero tindi ma Mbale kende ti lwoŋo ni Mbale Township District ti ketho Mr  Lukyn-Williams bedo District Commissioner mere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Thenge man ti lwoŋo ni Bugisu District, matero Bugisu gipi kod Sebei, aka Sazin aŋwen manitye iye; tiketho Mr Lindsell bedo District Commissioner mere</t>
+  </si>
+  <si>
+    <t>District machango oriwi i oro 1941, ti chwoko ni Mbale District, odoko opok kadi dek ka ndelo 4 November 1954; thenge man tilwoŋo ni Bukedi District matero Sazin awichiel; Pallisa, Budaka-Bugwere, Bunyole, West-Budama, Tororo kod Samia-Bugwe; tiketho Mr Dallimore bedo District Commissioner mere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rumachien to John Kakoro tich pere chungo, tidimo Yonasani Okello bedo ja Saza malunjo ka bedo pa John Kakoro, ka 1 July 1957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To munyo owir Yakobo Munabi tero go yo Saza ma Budaka-Bugwere kareno Danieri Nyapidi bende ti loko go bedo Deputy Judge ma District Native Court Bukedi, tidimo John Kakoro bedo ja Saza ka 1 January 1956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To munyo owir Danieri Nyapidi ka 1 January 1954 bedo ja Saza ma Samia-Bugwe ti wiro Yakobo Munabi lunjo ka bedo pere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Yo Saza ma East Budama, mati i lwoŋo ni Tororo ka 1 January 1949 tiketho Danieri Nyapidi lunjo ka bedo pa Temusewo Mukasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ka 13 October 1953 tiketho Zefaniya Ochieŋ bedo ja Saza, ama fuod dhumo kiri pama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Saza ma West Budama Andereya Ofumbi odhumo tundo 30 May 1953, to tho, munyo fuod dhumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ka 3 January 1947 to doko i poko adhum ma Padhola diryo West Budama tiketho Andereya Ofumbi bedo ja Saza mere, kod East Budama tiketho Temusewo Mukasa bedo ja Saza mere, to kareno kezekiya Okowu amukutho kuro kabedo no paa Acting</t>
+  </si>
+  <si>
+    <t>Paka gigipiny makite me nyaka chako moth moth, fuod derino mere kidwoŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Konyo dhano pajo kopodho iteko moro paka ma twech aka ongoye gilipya ma chulo, kiti ŋato nono choko rigo lipya tojogonyo go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nono meg jotyeko paro geto udi miten ma nono, fur famba manono kod oro kis janono bedo kod chiemo maromo mungoye kisaka asaka kis ndelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Paro kwom gigipiny makis ndelo, mamitere inono, paka: ketho chik manono, paro paka jonyalo dongo nono ikite machoko lipya paka mafwonjo gine nyithindho majochand, i nono pajo</t>
+  </si>
+  <si>
+    <t>Kod banjin moro gye minyalo tero iwaŋ jadwoŋ nono, rupir nitye banjin makikuthi chak ikooti ma gavumenti kwanyo woko koluwo ikooti ma nono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Banjin ma kite me ilwoŋo ni banjin, malusa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Joma kite me jo chulo dhiaŋ kod rombo ma luk; ruman odoko jo chulo kir lipya bende, gigipiny mi chulo no nono amachamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Thumo banjin banjin ma dudi ma nono, banjin mamako kwom pecho ma nitye iye dhaw dhaw kod kwerirok degi,  banjin ma pa jomo nywomere wat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To madwoŋ, jo temo tito swa gikikaŋasa gimo neko dhano pa jo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jodimo ŋata olunji dhako kosa mon pa ŋato, ka dhako no kosa mon no bende jo yeyere gi jo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jo chulo banjini munwaŋo ŋato nitye gine wok kwom pesa makaliel kosa gigipinyi pa ŋato, kendo jo pido banjin munwaŋo ŋato banja ji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Joketho misika pa ŋato, to ka misika no fuod thi jo dimo ŋata nyalo kuro pecho no milwoŋo ni Japith, makuro tundo kuma misika odongi iiye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kendo kaŋata otho obedo jachwo majapecho, nono chokere to jo yiko pecho majalo oweyo</t>
+  </si>
+  <si>
+    <t>Kony kadhano pajo otho: Ka dhano otho nono kosa wati paŋato kod merin pere gye, choko pesa kosa lim man gye mayii ŋato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Riwo nono kanyachiel: Jadwŋ nono choko ji to jo paro wach paka jonyalo riwirok kanyachielod ŋeyirok wegi gi wegi rupir mati me nono oasa pokirok pokirok iyadech mumore omore, riwirok makite me konyo igeŋo ji nywomirok wati kendo miyo nono ŋeyo welo pajo kod ŋeyo ji pajo majo tho</t>
+  </si>
+  <si>
+    <t>Tich ma jodongo nono jotimo nitye ama:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka nitye bitawin bende ma Jadwoŋ nono kano, manono jondiiko iiye gigipiny majoparo kwome ka jochokere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kis Jadwoŋ nono nitye gi jandiiko kodi jakan lipya manono; ma nono dimo jo ni jokonyigo gitich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ka Jadwoŋ nono otho kosa nono oryiemo go bedo jadwoŋ, nono chokere to odoko jo dimo ŋatiman</t>
+  </si>
+  <si>
+    <t>Indir me, kis nono nitye kod jadwoŋ mere matero nono gipi meno ti jolwoŋo ni Jasaza ma nono aka nitye ma jolwoŋo ni Jagombila, Jamiluka kod Jakisoko mabende jokidho kajotero adech mathindho thindho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka nonini meg mudoŋ jo asa chako ketho jodongo pajo i oro 1945, indir ma gavumenti okwayo ni kis nono odhir jadwoŋ mere kidho i chokirok ma kansolo mar'adhum; kiri pama gavumenti fuod yeyere kod tich pa jodongo nonini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To wok oro 1935 nonini madit jo chako ketho jodongo makite no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Paka Jopadhola jo kimit mako kula pa joman majowiloka piyopiyo mafuod jo kokaŋasa kulano maber, bende jokorikin dimo jodongo nonini mapiyopiyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ra' meno to wabende wachako ketho jo dongo manono gipi ikabedo ma ketho jodongo udi kende paka nyachoni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jotito riwan paka yo pajo koro kis nono nitye kod jadwoŋ mere kosa ja tel matero nono gipi</t>
   </si>
 </sst>
 </file>
@@ -576,7 +978,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -613,6 +1015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1741,10 +2144,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A23"/>
+  <dimension ref="A2:A157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1862,6 +2265,676 @@
         <v>163</v>
       </c>
     </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
at 343 additions and 100O left-History
</commit_message>
<xml_diff>
--- a/History and customs of Jopadhola.xlsx
+++ b/History and customs of Jopadhola.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="486">
   <si>
     <t xml:space="preserve">WACH MA CHAKO </t>
   </si>
@@ -930,6 +930,564 @@
   </si>
   <si>
     <t xml:space="preserve">  Jotito riwan paka yo pajo koro kis nono nitye kod jadwoŋ mere kosa ja tel matero nono gipi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Amor Kagulu Adundo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ri ameno to jo chako kwedirok, joman jo wacho ni wan wa jo paŋadin riwan, wakiya?ere gi win, kada nono, wakinono giwin; aka joman bende jo wacho ameno; to wok ruwirok madwoŋ kod pokirok nono kad bich paka onyo nitye pama</t>
+  </si>
+  <si>
+    <t>Pokirok manitye pama obedo riwach madhaw dhaw, kendo riwach munyo ka jo neko lee madwo? kosa dhia? pok mere kirom jo gye</t>
+  </si>
+  <si>
+    <t>Nywolirok pa nono me obedo ama (boli mucher me nyutho paka nywolirok me obedo wok kwom Adhola tundo, kwom kis jang nono Amor):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka kada jo pokere, fuod nitye wer, kweer, kod nyingi jo madit muriwojo</t>
+  </si>
+  <si>
+    <t>Nono Amor kada ti jo pokere kad bich aka odoko jo nywomere, chango jo gye baa jo achiel kende</t>
+  </si>
+  <si>
+    <t>NONO AMOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka Jadwoŋ nono pajo marapena jodimo i Apuli 1945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Yikirok pajo joyikere wiyijo ŋiyo yo thenge ma yo Sudan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  KUNU pajo nitye yo Senda ilul milwo?o ni Pawamunju</t>
+  </si>
+  <si>
+    <t>Tich ma yado jo asa ŋeyirok iiye: lweny kod goyo fumbo ma kosio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To indir mati me jo wero iyawo rut kosa ikalima morogye kod ikaliel pa dhano pajo</t>
+  </si>
+  <si>
+    <t>Wer aryo me gye yado jo wero yo lweny kod yo dwar</t>
+  </si>
+  <si>
+    <t>Jo p'Agoya mamako mon yokulo</t>
+  </si>
+  <si>
+    <t>Wer me jowero ka jo nyutho ni kada nende jo nok, chango jo konyalo tho jo gye i lweny, ni yado kajokidho lweny jo gye jo dwoko riwach misen pajo</t>
+  </si>
+  <si>
+    <t>ŋanda wambwe jo p'Agoya nyaka dwoko</t>
+  </si>
+  <si>
+    <t>Nono me ongoye kod kweer moro gye, yawo rut, kod paka minyur pa jo wok, kod kula manywomirok machon gye jotimo paka jo Padhola gye jotimo (nen Adech III)</t>
+  </si>
+  <si>
+    <t>Nyakawenga, Juri, Wiye Owaŋ, Oriŋo, Mbedi, Odida</t>
+  </si>
+  <si>
+    <t>Agoya,	Okidi,	Ondaga,	Ochomi,	Osuya,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nyingijo madongo, mati jo chwokere gine ame:</t>
+  </si>
+  <si>
+    <t>Jo p'Agoya jo dit iyadech milwoŋo ni Pagoya chiegin Nagongera, kodi yoloka pagoya man yo Kamuli, i Gombila ma Molo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Yach me amabende jonywolo nono me paka onyo nitye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka Nyakigulu me gi dhako pere milwoŋo ni Abwor amajo nywolo yach aŋwen, Juri, Okidi, Mbedi kod Ondaga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Agoya chango onywolo nyath achiel kende manyiyach milwoŋo ni Nyakigulu</t>
+  </si>
+  <si>
+    <t>Agoya chango obedo wod Adhola, aka go no am'onywolo nono me munyo lwoŋere ni jo p'Agoya</t>
+  </si>
+  <si>
+    <t>NONO JO P'AGOYA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To parere ni tundo yomalo koro gigipiny me bino dongo malo swa rupir kis dhano mito kendo sangala ritim maber manono pere timo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka odoko nono meg amo ayi iiye malo loyo meg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Minyur kod nyath jo nindo i boke pendi Nyarwanda ako odoko minyur no chiemo ikor pendi, kendo kiyik mach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Jo kited kod yath milwŋo ni Obolo</t>
+  </si>
+  <si>
+    <t>Jo kited kod yath milwoŋo ni Obolo</t>
+  </si>
+  <si>
+    <t>Kijwala,	Sanga,	Nyabel,	Miyali,	Kawudo,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nyingi jo madongo mati jo chwoko ame:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wugo pajo nitye Mikwana, me nyutho ni indir ma lweny pa Josewe kareno jotyeko tundo i kabedo no</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jo chako bedo iyadech ma Mikwana, kod Nagongera, akanyaka jolak i Padhola gye</t>
+  </si>
+  <si>
+    <t>Nono me nyingi jo man jowacho ni, "Wa jo pa Kijwala wodi Akwoyo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Amor Kijwala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  KUNU pajo achiel nitye Katajula itele milwoŋo ni Katajula, aka man nitye Maundo itele milwoŋo ni 'Tawo Jwok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka tich machango jo asa ŋeyirok iiye: lweny, timo riji yen (boke) matipo kod yen ma migimba koth, pach kod chuech</t>
+  </si>
+  <si>
+    <t>Jadwoŋ nono me marapena odim go i oro 1945</t>
+  </si>
+  <si>
+    <t>Ajore Kagulu Adundo nyaka wabino</t>
+  </si>
+  <si>
+    <t>Ondhiri wajocham malo nok nok</t>
+  </si>
+  <si>
+    <t>Ee, Kagulu Adundo nyikway Njose Kayoro</t>
+  </si>
+  <si>
+    <t>Wer pajo majo wero:</t>
+  </si>
+  <si>
+    <t>Jo yikere wiyijo ŋiyo yokuma waŋ chieŋ podho iy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Minyur kiyik mach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Minyur chiemo i kor pendi nyarwanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Minyur kod nyath jo nindo i boke pendi nyarwanda kanyath manyako, to ka majachwo jo nindo i boke nyameji</t>
+  </si>
+  <si>
+    <t>Jo kited kod yen aŋwen me: Kudho Alwi, Kagino, Obolo, kod Dukino Ath</t>
+  </si>
+  <si>
+    <t>Kweer pajo:</t>
+  </si>
+  <si>
+    <t>Njwaya,	Aaŋa,	Omunyi,	Sar,	Adusa</t>
+  </si>
+  <si>
+    <t>Okonye,	Masanja,	Otwepe,	Nyagota,	Nyanjoli,</t>
+  </si>
+  <si>
+    <t>Kitheŋi,	Misyoŋo,	Ogesi,	Otyemi,	Paliwo,</t>
+  </si>
+  <si>
+    <t>Kamunyi,	Oriono,	Moyi,	Oda,	Mweye,</t>
+  </si>
+  <si>
+    <t>Njose,	Luaŋole,	Ochido,	Alosi,	Wambiri,</t>
+  </si>
+  <si>
+    <t>Aka nyingi jo madongo mati jo chwoko ame:</t>
+  </si>
+  <si>
+    <t>Nono me jo chako bedo Katajula, chiegin Nagongera, akanyaka jo wok kenyo jolak i Padhola gipi, Nyingi jo man, jowacho ni "Wa jo kagulu Adundo wa nyikway Njose wa jo cham malomalo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Minyur chiemo imatigija pendi, kendo inywol makayo dhako kiyik mach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Minyur kod nyath jo nindo iboke pendi Nyarwanda kanyath manyako, aka nyameji kanyath manyiyach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Milusa kod obolo jo kited gine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Rudina jo kicham, kada geyo pyen mere jo kigey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Kweer madwo? Sulwe, ama jo chowo kendo joyiko ji wiyijo ?iyo yo Sulwe</t>
+  </si>
+  <si>
+    <t>Kweer pajo :</t>
+  </si>
+  <si>
+    <t>Langa,	Omolo,	Mawungwe,	Mumwara</t>
+  </si>
+  <si>
+    <t>Aliko, Magala, Kenga,Aryoŋa,Omo</t>
+  </si>
+  <si>
+    <t>Migwat,	Kidyewo,	Mugweno,	Kasinda,	Sulwe,</t>
+  </si>
+  <si>
+    <t>Adhola,	Okuna,	Obukumer,	Olebe,	Nyasulwe,</t>
+  </si>
+  <si>
+    <t>Asipa,	Mŋor,	Kisito,	Omoŋor,	Adusa,</t>
+  </si>
+  <si>
+    <t>Aka nyingijo madongo mati jo chwoko ame:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nyingi jo man jowacho ni "Wan Amor Adhola pa Tikidiegi Sulwe"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Chango jo chako bedo iyadech ma Nagongera kod yo Nyamalogo, rumachien to jo lak i Padhola gye</t>
+  </si>
+  <si>
+    <t>Jo pa Tikidiegi jo wacho ni jo ajo madwoŋ ajo ma telo Padhola gipi rupir nijo chowo kunu milwoŋo ni Adhola, kendo jowacho ni chango omiyijo Toŋ kod Buli p'Adhola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Amor pa Tikidiegi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  KUNU pajo nitye yo Simwengi, manago tele milwoŋo bende ni Simwengi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka tich machango jo asa ŋeyirok iiye: lweny, chuech kod pach</t>
+  </si>
+  <si>
+    <t>Jadwoŋ nono me marapena chango odim go i oro 1938</t>
+  </si>
+  <si>
+    <t>Piny p'Olam, Oryaŋ, piny pa Dundo Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t>Won piny aŋ Oryaŋ, won piny ŋaŋ Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t>Nyajurirya oo, oo, Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t>Jamor kokidho lweny kidwok nono</t>
+  </si>
+  <si>
+    <t>Gero, Gero, wajo Simwengi wakilwor chwo,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Jo yikere wiyijo neno kumwaŋ chieŋ odho iye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Minyur kod nyath jo nindo i boke pendi nyarwanda aka chiemo bende chiemo ikor pendi nyarwanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Kweer madoŋ Rudina, jo kicham, kada geyo pyen mere jo kigey</t>
+  </si>
+  <si>
+    <t>Mileke,	Orukan,	Ndelo,	Opusi,	Obilo</t>
+  </si>
+  <si>
+    <t>Aliŋa,	Olam,	Malawa,	Olyeka,	Adundo,</t>
+  </si>
+  <si>
+    <t>Aka nyingi jo madongo mati jochwoko ame:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nyingijo man jo wacho ni "Wa jo p'Olam Nyajurirya Oryaŋ Oryaŋ weg piny</t>
+  </si>
+  <si>
+    <t>Jo p'Olam chango jo chako bedo iyadech milwoŋo Simwengi, i Gombila ma Nagongera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Amor p'Olam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  KUNU pajo nitye mikwana manago obedo lul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka tich machango jo asa ŋeyirok iiye ame: lweny kod goyo achiel kod tida</t>
+  </si>
+  <si>
+    <t>Jadwoŋ nono pajo marapena oketh i oro 1947</t>
+  </si>
+  <si>
+    <t>Adech marapena mawer me jo tito ka jo poyo lweny machon, mayado kadhano ringo jokwor, ringo ŋiyo yoŋeye; kendo ni kadhano mito wacho nyingi nyawote okutho bolo waŋe yongeye onen ni ŋato ongoye kenyo akanyaka oluw</t>
+  </si>
+  <si>
+    <t>Kapanyi oywak wor wor ja Simba konwaŋ muthieno</t>
+  </si>
+  <si>
+    <t>Ee, Kijwala wod Akwoyo nen yoŋeyin</t>
+  </si>
+  <si>
+    <t>Jo yikere wiyijo ŋiyo kuma waŋ chieŋ podho iy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bendo onywolo wode milwoŋo ni Sole, aka Sole onywolo Milwen, aka Milwen onywolo yach apar gabich, yach me ama jo nywolo nono Bendo gye manitye pama</t>
+  </si>
+  <si>
+    <t>Bendo munywolo nono jo pa Bendo, chango wod Adhola</t>
+  </si>
+  <si>
+    <t>NONO JO PA BENDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  KUNU pajo nitye Nyamalogo itele milwoŋo ni Mugulu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tich machango jo asa ?eyirok iiye: lweny, dwaŋ  kod goyo Achie1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To chango chon oyido jo nitye kod jo dongo aryo, achieŋ mayo thenge pa Mugulu kende aka man mayo thenge pa Kasede bende kende</t>
+  </si>
+  <si>
+    <t>Jadwoŋ nono me marapena mariwo jo gye oketh i oro 1954</t>
+  </si>
+  <si>
+    <t>Piny weg, Oryaŋ, piny Amor Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t>Piny Mugulu, Oryaŋ, piny Kasede Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oryaŋ, won piny ŋa? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Won piny ŋa?   </t>
+  </si>
+  <si>
+    <t>Nyajurya oo, oo, Oryaŋ Oryaŋ</t>
+  </si>
+  <si>
+    <t>Nyajurya oo, oo, Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Jo yikere wiy jo ŋiyo kuma waŋ  chieŋ podho iye </t>
+  </si>
+  <si>
+    <t>Yen Ragadhiŋ, Akibuk kod Okwero, jo kited gine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Minyur chiemo ikor pendi, kiyik mach, kendo kikyeg thigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 	Kweer madwoŋ Rudina, jo kicham kada geyo yer mere kosa pyen jo kigey</t>
+  </si>
+  <si>
+    <t>Kasede</t>
+  </si>
+  <si>
+    <t>Kayoro,	Obwaga,	Achiero,	Achiko,	Ochakazi,</t>
+  </si>
+  <si>
+    <t>Mikwaya,	Nyambiro,	Okeji,	Kamunyi,	Akanga,</t>
+  </si>
+  <si>
+    <t>Okonye, Mawuya, Ochor, Asyaŋa, Apuw</t>
+  </si>
+  <si>
+    <t>Nyingi jo man jowacho ni, "waŋ  Amor Mugulu-Kasede, Nyajurya Oryaŋ weg piny"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tundo ka ndelo 10 October 1954 aka jo chokere to jo ridho ni wangi olwoŋo jo ni Amor Mugulu-Kasede, indelo no bende amajo dimo iye Jadwoŋ achieŋ ma riwo jo gye</t>
+  </si>
+  <si>
+    <t>Nono me wok chon jotemo paka jowir nyingi jo obed achieŋ kende, ikabedo mawacho ni Amor Kasede, Amor Mugulu; to jo koyeyere rupir Kasede mito ni apere amuwinjere malo, aka Mugulu bende mito ni apere amonek apa Kasede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To Kasede nyinge oasa winjirok ri waŋ  tek pere kendo ri ŋiyo pere; Mugulu chango obedo jagwondo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kendo go ama Jadwoŋ pa Kasede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mugulu nyinge won chango ilwoŋo ni Kayoro to ri chowo mago chango chowo Kunu milwoŋo ni Mugulu yo Nyamalogo amuŋiyo owir nyinge ni Mugulu</t>
+  </si>
+  <si>
+    <t>Paka nende waneno ikachako ma Siro me, Mugulu kod Kasede jo wutimere, ma ich achiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Amor Mugulu-Kasede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mararyo nitye Nyamalogo manago tele majo lwoŋo ni Adhola nitye iwiyi got Nyamanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  KUNU, pajo nitye aryo madwoŋ mere Sulwe Manyichwo jo lwoŋo Rwoth Sulwe, aka dhako pere jo lwoŋo Michala Sulwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tich machango jo asa ŋeyirok iiye: lweny, kwoyo kwoot kod goyo Achiel</t>
+  </si>
+  <si>
+    <t>Jadwoŋ nono me marapena chango oketh i oro 1936</t>
+  </si>
+  <si>
+    <t>Piny Adhola, Oryaŋ, piny Sulwe Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t>Won piny ŋaŋ  Oryaŋ, won piny ŋaŋ Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t>Won piny ŋaŋ  Oryaŋ, Oryaŋ</t>
+  </si>
+  <si>
+    <t>Jo yikere wiyijo ŋiyo Sulwe yo thenge ma Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jo pa Bendo nyingi jo man ma jo pakere gine jowacho ni, "Wa jo Goryaŋ waŋ  Ogwaŋ  Ayese"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ka nyathi munywolino manyichwo bende iŋiyo pig sikondi manyichwo, ka ma nyako iŋiyo sikondi madhako</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Iŋiyo pig Sikondi inyuka paminyur akanyaka minyur madho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Dukino Athu amiguro gine nyuka pa minyur, kareno otwey sikondi yowiy alikino dukino no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Nyuka maminyur madho, kitwaŋ  ikendo, amuŋiyo itedo nyakamathi kachiegin twaŋ  titiŋo woko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Oti minyur kiywey tundo kuma minyur wok iye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nyuka kende amamadho aka nyuka no bende go won kimak gichinge kwanyo woko imiy'amiya go idhoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Kadhako onywol kimadh pii tieko ndelo adek konywolo nyiyach aka ndelo aŋwen konywolo nyako</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Yath milwoŋo ni kikwala kited gine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nyingi jo mati jochwoko ame:</t>
+  </si>
+  <si>
+    <t>Iyadech machango jo asa dit iye Maundo, Paya kod Kirewa akanyaka jolak i Padhola gye</t>
+  </si>
+  <si>
+    <t>Biranga me nyingi jo man majo pakere gine jowacho ni, "Wa jo p'Owiny kosa Wa jo p'Ariko, wakilwor Moryeko"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Biranga Owiny kod p'Ariko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To kada nende pama jo pokere, kweer megi kodi nyingijo madit chale, meno nyutho ni nonin adek me chango achiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biranga Nyakaŋo kod'Abwor, kodi </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> biranga Owinyi kod p'Ariko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nyithindho me gye bende to jonyayi jangijo munyo jorwenyo swa kiri nywomirok gye jo nywomere, to doko bino riwirok moro ka jangijo madongo joriwere ka jolwoŋere ni wajo pa ŋadin akuma onyo owok iye jange adek madongo munyo pama nitye: </t>
+  </si>
+  <si>
+    <t>Nyithindho pa Masawa ame:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rumachieŋ towok iye nonin madongo aryo: Biranga kod Ragaŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To Masawa obedo kod mon kweth yee to nywolo yach kweth swa aka yach me riwach madhaw dhaw paka asa bedo inyithindho ma jo poko minigin, ndir madit jo kimitere, amuŋiyo nyithindho pa Masawa jopokere tek tek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Masawa me onywol go rut kod Agak (nen Siro 5 Ragaŋ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tiend nonin me chango ochakere ama: Adhola amunywolo dhano milwoŋo ni Omolo aka Omolo kod dhako pere milwoŋo ni Luya, jonywolo nyiyach milwoŋo ni Masawa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ŋeyo paka pokirok obedo maDwoŋ   neni kiri Biranga won odoko opokere ka di kweth</t>
+  </si>
+  <si>
+    <t>Nono Biranga kod nono Ragaŋ baa jo achieŋ to ri pokirok mubedo chon swa onyo pama nonin me jokiŋey ni chango jowutimere kada dichiel</t>
+  </si>
+  <si>
+    <t>NONO JO BIRANGA KOD JO PA RAGAŋ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  JaDwoŋ   nono pajo marapena chango jo dimo i oro 1923</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jo nitye kod KUNU adek, maDwoŋ   mere 'Okita' nitye Nagongera; man nitye Nyamalogo iwiy got milwoŋo ni Nyamanda; maradek nitye Maundo manago tele milwoŋo ni 'Wagitoko</t>
+  </si>
+  <si>
+    <t>Tich machango nono me oasa ŋeyere iiye: lweny, dwar, goyo fumbo, tongoli kod bunde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wer me iwero i lweny, ika liel, kod i rut</t>
+  </si>
+  <si>
+    <t>Me awer majo wero ka jopako misen pajo, jo p'Ogwaŋ  Ayese jo Bendo jo kilwor Jowi</t>
+  </si>
+  <si>
+    <t>Awuyo Ogwaŋ  Ayese kilwor Jowi</t>
+  </si>
+  <si>
+    <t>Awuyo wanyithindho awuyo Sambara</t>
+  </si>
+  <si>
+    <t>Wer pajo jo wero ni:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Jo yikere wiyijo neno yokuma waŋ  chieŋ woki iye </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Dukino mu bokere bende ikelo boke mere adek kanyath no ma nyiyach kosa boke aŋwen ka ma nyako, tichomo inyim dhioti akanyaka dhako no chiemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To kudho alwino minyur no kicham kwanyo woko chungo achunga kenyo ma kweer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ikelo kudho alwi tichomo inyuka maminyur yamadho kosa ikwon mayachamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Kaminyur yawok, indir mitedo iye kwon apipili (nen Adech III, Siro 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Yen milwoŋo ni kudho Alwi, kod Ragadhiaŋ  kited gin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Manyutho ni chiemo marapena, kandelono orumo anyuka no ma sikondi bino thon iye</t>
+  </si>
+  <si>
+    <t>Ka dhako onywol tieko ndelo adek kanyath no ma nyiyach, aka ka ma nyako tieko ndelo aŋwen, mafuod kochiemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kakobedo ameno nyutho ni nyath no kobed gisilwany maber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ka dhako onywol sikondi bino abina to thono pige inyuka muted ri dhako maminyur, aka nyaka dhako no madho</t>
+  </si>
+  <si>
+    <t>Kweer pa nono Bendo madwoŋ  SIKONDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ndiri munyo Oguti odongo, Milwen onywomo rigo mon adek, Abotha nya ja Ramogi, Nyagol kod Nyakuya nyir Morwa Sule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Milwen chango oketho Oguti ioti pa dhako pere milwoŋo ni min Owaro, kenyo ama odongo iiye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ja pa Bendo milwoŋo ni Milwen amonwaŋo Oguti iger dhok, ikabedo ma Pokoŋo Nagongera, tokelo go pecho pere toloko go panyath pere</t>
+  </si>
+  <si>
+    <t>I non Bendo me amachango jali milwoŋo ni Oguti odonjo iiye (nen Adech I, Siro 3)</t>
+  </si>
+  <si>
+    <t>Sole, Aŋwela, Oguti, Ogola, Ochol, Milwen, Owaro, Obyeto</t>
+  </si>
+  <si>
+    <t>To kareno onyo jolaki i Padhola gipi</t>
+  </si>
+  <si>
+    <t>Nono me ochako bedo iyadech ma Nagongera, Tororo kod Kwapa, kiripama akuma jo asa more iye tek tek</t>
+  </si>
+  <si>
+    <t>Dwoŋ  mere ni jo joger swa aka chango jo mako kir ogwange madongo, kokwinyo jo</t>
   </si>
 </sst>
 </file>
@@ -978,7 +1536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1016,6 +1574,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2144,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A157"/>
+  <dimension ref="A2:A343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="H121" sqref="H121"/>
+    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
+      <selection activeCell="E328" sqref="E328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2935,6 +3494,936 @@
         <v>275</v>
       </c>
     </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1">
+      <c r="A270" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1">
+      <c r="A271" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1">
+      <c r="A272" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1">
+      <c r="A273" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1">
+      <c r="A275" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1">
+      <c r="A276" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1">
+      <c r="A277" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1">
+      <c r="A280" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1">
+      <c r="A281" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1">
+      <c r="A282" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1">
+      <c r="A283" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1">
+      <c r="A284" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1">
+      <c r="A285" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1">
+      <c r="A286" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1">
+      <c r="A287" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1">
+      <c r="A288" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1">
+      <c r="A289" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1">
+      <c r="A290" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1">
+      <c r="A291" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1">
+      <c r="A292" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1">
+      <c r="A293" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1">
+      <c r="A294" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1">
+      <c r="A295" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1">
+      <c r="A296" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1">
+      <c r="A297" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1">
+      <c r="A298" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1">
+      <c r="A299" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1">
+      <c r="A301" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1">
+      <c r="A302" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1">
+      <c r="A303" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1">
+      <c r="A304" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1">
+      <c r="A305" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1">
+      <c r="A306" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1">
+      <c r="A307" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1">
+      <c r="A308" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1">
+      <c r="A309" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1">
+      <c r="A310" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1">
+      <c r="A311" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1">
+      <c r="A312" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1">
+      <c r="A313" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1">
+      <c r="A314" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1">
+      <c r="A315" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1">
+      <c r="A316" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1">
+      <c r="A317" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1">
+      <c r="A318" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1">
+      <c r="A319" s="15" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1">
+      <c r="A320" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1">
+      <c r="A321" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1">
+      <c r="A322" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1">
+      <c r="A323" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1">
+      <c r="A324" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1">
+      <c r="A325" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1">
+      <c r="A326" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1">
+      <c r="A327" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1">
+      <c r="A328" s="14" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1">
+      <c r="A329" s="14" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1">
+      <c r="A330" s="14" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1">
+      <c r="A331" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1">
+      <c r="A332" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1">
+      <c r="A333" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1">
+      <c r="A334" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1">
+      <c r="A335" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1">
+      <c r="A336" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1">
+      <c r="A337" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1">
+      <c r="A338" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1">
+      <c r="A339" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1">
+      <c r="A340" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1">
+      <c r="A341" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1">
+      <c r="A342" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1">
+      <c r="A343" t="s">
+        <v>435</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>